<commit_message>
menambahkan fitur invoice, penyesuaian kode
</commit_message>
<xml_diff>
--- a/tes_import.xlsx
+++ b/tes_import.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="111">
   <si>
     <t xml:space="preserve"> 3D Bowknot Smile Lucky Cat Cartoon Silicone Cases Cover </t>
   </si>
@@ -162,9 +162,6 @@
 Fast Response WA : 08980085967</t>
   </si>
   <si>
-    <t>TP169849484</t>
-  </si>
-  <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2017/4/5/915535/915535_fbd17524-a37d-4ca3-b3ab-d82650eb88e3.jpg</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>3D Silicone Cartoon</t>
   </si>
   <si>
-    <t>TP43713645</t>
-  </si>
-  <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2016/5/14/7654834/7654834_e4871e3d-16df-42fa-b775-b78603209249.jpg</t>
   </si>
   <si>
@@ -201,18 +195,12 @@
     <t>Asus Zenfone 2 5.5 ZE551ML ACC</t>
   </si>
   <si>
-    <t>TP142250063</t>
-  </si>
-  <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2016/8/8/55148722/55148722_4025b071-b7d3-444a-a7d3-05957d97448c.jpg</t>
   </si>
   <si>
     <t>TEMPERED GLASS</t>
   </si>
   <si>
-    <t>TP43713277</t>
-  </si>
-  <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2016/5/14/7654834/7654834_4ec66048-51f5-48a7-a60c-662996125a16.jpg</t>
   </si>
   <si>
@@ -231,22 +219,13 @@
     <t>Zenfone Selfie ACC</t>
   </si>
   <si>
-    <t>TP40209157</t>
-  </si>
-  <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2016/4/16/7654834/7654834_be958023-6d53-4e39-a48d-a054ee9219b1.jpg</t>
   </si>
   <si>
-    <t>TP100410286</t>
-  </si>
-  <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2016/11/27/7654834/7654834_dd82eab4-9c37-4e4a-8358-592a5e7828fb_960_960.jpg</t>
   </si>
   <si>
     <t>SAMSUNG A3 ACC</t>
-  </si>
-  <si>
-    <t>TP37964482</t>
   </si>
   <si>
     <t xml:space="preserve"> Galaxy A3 2016 A310 Aluminum Metal Bumper Mirror Hard Back Case </t>
@@ -278,9 +257,6 @@
     <t>https://ecs7.tokopedia.net/img/product-1/2016/3/29/7654834/7654834_e747670f-01c1-4787-b074-28383767ea7e.jpg</t>
   </si>
   <si>
-    <t>TP35999959</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Galaxy A3 A300 Aluminum Metal Bumper Mirror Plating Hard Back Case </t>
   </si>
   <si>
@@ -310,9 +286,6 @@
   </si>
   <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2016/3/12/7654834/7654834_f350a7d7-974e-43f3-9d96-8b6b0fb62ec8.jpg</t>
-  </si>
-  <si>
-    <t>TP85839241</t>
   </si>
   <si>
     <t xml:space="preserve"> Galaxy A310 2016 Smart Flip Slim View Electroplating Mirror Hard Case </t>
@@ -356,9 +329,6 @@
     <t>https://ecs7.tokopedia.net/img/product-1/2016/11/2/7654834/7654834_174b24ad-5963-4ec4-be7b-8b0528b7e688.jpg</t>
   </si>
   <si>
-    <t>TP100410610</t>
-  </si>
-  <si>
     <t xml:space="preserve"> GALAXY A5 2016 A510 3D Cute Cartoon Sulley Case Soft Silicon Case </t>
   </si>
   <si>
@@ -366,9 +336,6 @@
   </si>
   <si>
     <t>SAMSUNG A5 ACC</t>
-  </si>
-  <si>
-    <t>TP48639524</t>
   </si>
   <si>
     <t xml:space="preserve"> Galaxy A7 2016 A710 Colorful Tempered glass gold </t>
@@ -410,9 +377,6 @@
     <t>SAMSUNG A7 A710 ACC</t>
   </si>
   <si>
-    <t>TP36000964</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Galaxy A7 A710 Aluminum Metal Bumper Mirror Plating Hard Back Case </t>
   </si>
   <si>
@@ -448,9 +412,6 @@
     <t>https://ecs7.tokopedia.net/img/product-1/2016/3/12/7654834/7654834_b0d2c0e6-c43c-44d4-84fd-40fded95fb0d.jpg</t>
   </si>
   <si>
-    <t>TP34065088</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Galaxy A8 Aluminum Metal Bumper Mirror Plating Hard Back Case </t>
   </si>
   <si>
@@ -483,9 +444,6 @@
   </si>
   <si>
     <t>SAMSUNG A8 ACC</t>
-  </si>
-  <si>
-    <t>TP109053512</t>
   </si>
   <si>
     <t xml:space="preserve"> Galaxy A9 PRO Smart Flip Slim View Electroplating Mirror Hard Case </t>
@@ -533,9 +491,6 @@
     <t>SAMSUNG A9 ACC</t>
   </si>
   <si>
-    <t>TP39681981</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Galaxy E5 E500 Aluminum Bumper Mirror Hard Back Case </t>
   </si>
   <si>
@@ -567,9 +522,6 @@
   </si>
   <si>
     <t>SAMSUNG E5 ACC</t>
-  </si>
-  <si>
-    <t>TP39682340</t>
   </si>
   <si>
     <t xml:space="preserve"> Galaxy E7 Aluminum Bumper Mirror Hard Back Case </t>
@@ -605,9 +557,6 @@
   </si>
   <si>
     <t>SAMSUNG E7 ACC</t>
-  </si>
-  <si>
-    <t>TP35523793</t>
   </si>
   <si>
     <t xml:space="preserve"> GALAXY GRAND 2 G7102 G7106 TEMPERED GLASS 0.26 mm / 2.5D 9H </t>
@@ -638,9 +587,6 @@
   </si>
   <si>
     <t>SAMSUNG GRAND 2 / G7106 / G7102 ACC</t>
-  </si>
-  <si>
-    <t>TP48639176</t>
   </si>
   <si>
     <t xml:space="preserve"> Galaxy Grand Prime G530 / G531 Colorful Tempered glass gold </t>
@@ -682,9 +628,6 @@
     <t>SAMSUNG GRAND PRIME ACC</t>
   </si>
   <si>
-    <t>TP88978946</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Galaxy Grand Prime G530 Silicone 3D Sulley Case Cover </t>
   </si>
   <si>
@@ -702,63 +645,6 @@
   </si>
   <si>
     <t>https://ecs7.tokopedia.net/img/product-1/2016/11/8/7654834/7654834_2d811b6a-34a5-4f79-9372-2295d697a452.jpg</t>
-  </si>
-  <si>
-    <t>TP169849484-1.jpg</t>
-  </si>
-  <si>
-    <t>TP43713645-1.jpg</t>
-  </si>
-  <si>
-    <t>TP142250063-1.jpg</t>
-  </si>
-  <si>
-    <t>TP43713277-1.jpg</t>
-  </si>
-  <si>
-    <t>TP40209157-1.jpg</t>
-  </si>
-  <si>
-    <t>TP100410286-1.jpg</t>
-  </si>
-  <si>
-    <t>TP37964482-1.jpg</t>
-  </si>
-  <si>
-    <t>TP35999959-1.jpg</t>
-  </si>
-  <si>
-    <t>TP85839241-1.jpg</t>
-  </si>
-  <si>
-    <t>TP100410610-1.jpg</t>
-  </si>
-  <si>
-    <t>TP48639524-1.jpg</t>
-  </si>
-  <si>
-    <t>TP36000964-1.jpg</t>
-  </si>
-  <si>
-    <t>TP34065088-1.jpg</t>
-  </si>
-  <si>
-    <t>TP109053512-1.jpg</t>
-  </si>
-  <si>
-    <t>TP39681981-1.jpg</t>
-  </si>
-  <si>
-    <t>TP39682340-1.jpg</t>
-  </si>
-  <si>
-    <t>TP35523793-1.jpg</t>
-  </si>
-  <si>
-    <t>TP48639176-1.jpg</t>
-  </si>
-  <si>
-    <t>TP88978946-1.jpg</t>
   </si>
 </sst>
 </file>
@@ -1100,10 +986,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1111,7 +997,7 @@
     <col min="4" max="4" width="74.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1125,31 +1011,28 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>130</v>
+        <v>12</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1163,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1174,17 +1057,14 @@
       <c r="H2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1198,19 +1078,16 @@
         <v>5</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1224,31 +1101,28 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>133</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1262,19 +1136,16 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1288,21 +1159,18 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="J6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B7">
         <v>25000</v>
@@ -1311,30 +1179,27 @@
         <v>100</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
-        <v>136</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>47</v>
       </c>
       <c r="B8">
         <v>25000</v>
@@ -1343,33 +1208,30 @@
         <v>100</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E8" t="s">
-        <v>137</v>
+        <v>41</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J8" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="K8">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B9">
         <v>57000</v>
@@ -1378,36 +1240,33 @@
         <v>130</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>138</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="H9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" t="s">
-        <v>60</v>
-      </c>
-      <c r="L9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>57000</v>
@@ -1419,21 +1278,18 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
-      <c r="L10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="J10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>40000</v>
@@ -1442,30 +1298,27 @@
         <v>100</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>140</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
-      <c r="I11" t="s">
-        <v>70</v>
-      </c>
-      <c r="L11" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B12">
         <v>25000</v>
@@ -1474,36 +1327,33 @@
         <v>100</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="F12" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="I12" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="J12" t="s">
-        <v>78</v>
-      </c>
-      <c r="K12" t="s">
-        <v>79</v>
-      </c>
-      <c r="L12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="K12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B13">
         <v>25000</v>
@@ -1512,33 +1362,30 @@
         <v>80</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>142</v>
+        <v>70</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
-      </c>
-      <c r="I13" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="J13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L13" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="K13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B14">
         <v>67000</v>
@@ -1547,36 +1394,33 @@
         <v>100</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="G14" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="H14" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="I14" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="J14" t="s">
-        <v>94</v>
-      </c>
-      <c r="K14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L14" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="K14">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="B15">
         <v>25000</v>
@@ -1585,33 +1429,30 @@
         <v>100</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G15" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="H15" t="s">
-        <v>101</v>
-      </c>
-      <c r="I15" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="J15" t="s">
-        <v>103</v>
-      </c>
-      <c r="L15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="K15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B16">
         <v>25000</v>
@@ -1620,33 +1461,30 @@
         <v>100</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="E16" t="s">
-        <v>145</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="G16" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="H16" t="s">
-        <v>109</v>
-      </c>
-      <c r="I16" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="J16" t="s">
-        <v>111</v>
-      </c>
-      <c r="L16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="K16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B17">
         <v>25000</v>
@@ -1655,24 +1493,21 @@
         <v>100</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
-      </c>
-      <c r="F17" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" t="s">
-        <v>116</v>
-      </c>
-      <c r="L17" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="J17" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="B18">
         <v>45000</v>
@@ -1681,30 +1516,27 @@
         <v>100</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="E18" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="F18" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="G18" t="s">
-        <v>121</v>
-      </c>
-      <c r="H18" t="s">
-        <v>122</v>
-      </c>
-      <c r="I18" t="s">
-        <v>123</v>
-      </c>
-      <c r="L18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="J18" t="s">
+        <v>106</v>
+      </c>
+      <c r="K18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B19">
         <v>57000</v>
@@ -1713,22 +1545,19 @@
         <v>100</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="E19" t="s">
-        <v>148</v>
+        <v>109</v>
       </c>
       <c r="F19" t="s">
-        <v>125</v>
-      </c>
-      <c r="G19" t="s">
-        <v>128</v>
-      </c>
-      <c r="H19" t="s">
-        <v>129</v>
-      </c>
-      <c r="L19" t="s">
-        <v>124</v>
+        <v>110</v>
+      </c>
+      <c r="J19" t="s">
+        <v>106</v>
+      </c>
+      <c r="K19">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>